<commit_message>
setting up self tests for simulation
</commit_message>
<xml_diff>
--- a/input/OM_EM_Scenarios.xlsx
+++ b/input/OM_EM_Scenarios.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE068A9E-0343-274F-93B5-FB4AD5E8CAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF2DB02-32DD-8944-BABD-F5C3B4B91A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="1600" windowWidth="28900" windowHeight="16940" activeTab="1" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
   </bookViews>
   <sheets>
     <sheet name="OM" sheetId="1" r:id="rId1"/>
-    <sheet name="EM" sheetId="2" r:id="rId2"/>
+    <sheet name="EM_Self_Tests" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>Fast_LL_DatLow</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>logistic,gamma</t>
+  </si>
+  <si>
+    <t>OM_Application</t>
+  </si>
+  <si>
+    <t>Fast_LL_DatLow,Fast_LL_DatHigh,Slow_LL_DatLow,Slow_LL_DatHigh</t>
+  </si>
+  <si>
+    <t>Fast_LG_DatLow,Fast_LG_DatHigh,Slow_LG_DatLow,Slow_LG_DatHigh</t>
   </si>
 </sst>
 </file>
@@ -543,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3458753E-37AB-3F45-AB3E-5A0862A1384B}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1223,10 +1232,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1151FF97-D0E1-0C4A-B3E8-5F557C369670}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1235,9 +1244,11 @@
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="24.5" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="61.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -1256,8 +1267,11 @@
       <c r="F1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1276,8 +1290,11 @@
       <c r="F2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1296,8 +1313,11 @@
       <c r="F3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1316,8 +1336,11 @@
       <c r="F4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1336,8 +1359,11 @@
       <c r="F5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1356,8 +1382,11 @@
       <c r="F6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1375,6 +1404,9 @@
       </c>
       <c r="F7" t="s">
         <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding simulation pltos, etc
</commit_message>
<xml_diff>
--- a/input/OM_EM_Scenarios.xlsx
+++ b/input/OM_EM_Scenarios.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3B4419-6605-9B45-B159-0EB9B34A3096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5B6888-F668-5B48-B811-EA362C0CB8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="1600" windowWidth="28900" windowHeight="16940" activeTab="1" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
   </bookViews>
   <sheets>
     <sheet name="OM" sheetId="1" r:id="rId1"/>
-    <sheet name="EM_Self_Tests" sheetId="2" r:id="rId2"/>
-    <sheet name="EM_Runs" sheetId="3" r:id="rId3"/>
+    <sheet name="OM_TestCases" sheetId="6" r:id="rId2"/>
+    <sheet name="EM_Self_Tests" sheetId="2" r:id="rId3"/>
+    <sheet name="EM_Runs" sheetId="3" r:id="rId4"/>
+    <sheet name="EM_Runs_TVCont" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="116">
   <si>
     <t>Fast_LL_DatLow</t>
   </si>
@@ -190,27 +192,18 @@
     <t>Term_1Fl_ExpL_TVBlk</t>
   </si>
   <si>
-    <t>Term_1Fl_ExpL_TVCont</t>
-  </si>
-  <si>
     <t>10_1Fl_ExpL_TI</t>
   </si>
   <si>
     <t>10_1Fl_ExpL_TVBlk</t>
   </si>
   <si>
-    <t>10_1Fl_ExpL_TVCont</t>
-  </si>
-  <si>
     <t>5_1Fl_ExpL_TI</t>
   </si>
   <si>
     <t>5_1Fl_ExpL_TVBlk</t>
   </si>
   <si>
-    <t>5_1Fl_ExpL_TVCont</t>
-  </si>
-  <si>
     <t>5_1Fl_L_TI</t>
   </si>
   <si>
@@ -223,21 +216,12 @@
     <t>Term_1Fl_L_TVBlk</t>
   </si>
   <si>
-    <t>Term_1Fl_L_TVCont</t>
-  </si>
-  <si>
     <t>10_1Fl_L_TVBlk</t>
   </si>
   <si>
-    <t>10_1Fl_L_TVCont</t>
-  </si>
-  <si>
     <t>5_1Fl_L_TVBlk</t>
   </si>
   <si>
-    <t>5_1Fl_L_TVCont</t>
-  </si>
-  <si>
     <t>ln_fish_selpars_re</t>
   </si>
   <si>
@@ -269,13 +253,148 @@
   </si>
   <si>
     <t>Fast_GL_DatLow,Fast_GL_DatHigh,Slow_GL_DatLow,Slow_GL_DatHigh</t>
+  </si>
+  <si>
+    <t>Term_1Fl_ExpL_TVCont_0.5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_L_TVCont_0.5</t>
+  </si>
+  <si>
+    <t>10_1Fl_ExpL_TVCont_0.5</t>
+  </si>
+  <si>
+    <t>10_1Fl_L_TVCont_0.5</t>
+  </si>
+  <si>
+    <t>5_1Fl_ExpL_TVCont_0.5</t>
+  </si>
+  <si>
+    <t>5_1Fl_L_TVCont_0.5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_ExpL_TVCont_1.0</t>
+  </si>
+  <si>
+    <t>Term_1Fl_L_TVCont_1.0</t>
+  </si>
+  <si>
+    <t>10_1Fl_ExpL_TVCont_1.0</t>
+  </si>
+  <si>
+    <t>10_1Fl_L_TVCont_1.0</t>
+  </si>
+  <si>
+    <t>5_1Fl_ExpL_TVCont_1.0</t>
+  </si>
+  <si>
+    <t>5_1Fl_L_TVCont_1.0</t>
+  </si>
+  <si>
+    <t>Sigma_Fixed</t>
+  </si>
+  <si>
+    <t>Term_1Fl_ExpL_TVCont_1.5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_L_TVCont_1.5</t>
+  </si>
+  <si>
+    <t>10_1Fl_ExpL_TVCont_1.5</t>
+  </si>
+  <si>
+    <t>10_1Fl_L_TVCont_1.5</t>
+  </si>
+  <si>
+    <t>5_1Fl_ExpL_TVCont_1.5</t>
+  </si>
+  <si>
+    <t>5_1Fl_L_TVCont_1.5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_ExpL_TVCont_2.0</t>
+  </si>
+  <si>
+    <t>Term_1Fl_L_TVCont_2.0</t>
+  </si>
+  <si>
+    <t>10_1Fl_ExpL_TVCont_2.0</t>
+  </si>
+  <si>
+    <t>10_1Fl_L_TVCont_2.0</t>
+  </si>
+  <si>
+    <t>5_1Fl_ExpL_TVCont_2.0</t>
+  </si>
+  <si>
+    <t>5_1Fl_L_TVCont_2.0</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_TI</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_TVBlk</t>
+  </si>
+  <si>
+    <t>10_1Fl_Gam_TI</t>
+  </si>
+  <si>
+    <t>10_1Fl_Gam_TVBlk</t>
+  </si>
+  <si>
+    <t>5_1Fl_Gam_TI</t>
+  </si>
+  <si>
+    <t>5_1Fl_Gam_TVBlk</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_TVCont_0.5</t>
+  </si>
+  <si>
+    <t>10_1Fl_Gam_TVCont_0.5</t>
+  </si>
+  <si>
+    <t>5_1Fl_Gam_TVCont_0.5</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_TVCont_1.0</t>
+  </si>
+  <si>
+    <t>10_1Fl_Gam_TVCont_1.0</t>
+  </si>
+  <si>
+    <t>5_1Fl_Gam_TVCont_1.0</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_TVCont_1.5</t>
+  </si>
+  <si>
+    <t>10_1Fl_Gam_TVCont_1.5</t>
+  </si>
+  <si>
+    <t>5_1Fl_Gam_TVCont_1.5</t>
+  </si>
+  <si>
+    <t>5_1Fl_Gam_TVCont_2.0</t>
+  </si>
+  <si>
+    <t>10_1Fl_Gam_TVCont_2.0</t>
+  </si>
+  <si>
+    <t>Term_1Fl_Gam_TVCont_2.0</t>
+  </si>
+  <si>
+    <t>ShortFast_LL_DatHigh</t>
+  </si>
+  <si>
+    <t>ShortFast_GL_DatHigh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -286,6 +405,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -631,7 +756,7 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G9"/>
+      <selection activeCell="A5" activeCellId="1" sqref="A3:XFD3 A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -871,7 +996,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -942,7 +1067,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -1155,7 +1280,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1226,7 +1351,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -1301,11 +1426,244 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79EC034-2FE7-9043-9DC4-2D3AB80C9B4B}">
+  <dimension ref="A1:W3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>0.108</v>
+      </c>
+      <c r="E2">
+        <v>1.08E-3</v>
+      </c>
+      <c r="F2">
+        <v>0.01</v>
+      </c>
+      <c r="G2">
+        <v>0.85</v>
+      </c>
+      <c r="H2">
+        <v>200</v>
+      </c>
+      <c r="I2">
+        <v>200</v>
+      </c>
+      <c r="J2">
+        <v>200</v>
+      </c>
+      <c r="K2">
+        <v>0.2</v>
+      </c>
+      <c r="L2">
+        <v>50</v>
+      </c>
+      <c r="M2">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2">
+        <v>4</v>
+      </c>
+      <c r="Q2">
+        <v>0.85</v>
+      </c>
+      <c r="R2">
+        <v>6</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>8</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2">
+        <v>10</v>
+      </c>
+      <c r="W2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>0.108</v>
+      </c>
+      <c r="E3">
+        <v>1.08E-3</v>
+      </c>
+      <c r="F3">
+        <v>0.01</v>
+      </c>
+      <c r="G3">
+        <v>0.85</v>
+      </c>
+      <c r="H3">
+        <v>200</v>
+      </c>
+      <c r="I3">
+        <v>200</v>
+      </c>
+      <c r="J3">
+        <v>200</v>
+      </c>
+      <c r="K3">
+        <v>0.2</v>
+      </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="M3">
+        <v>50</v>
+      </c>
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>6</v>
+      </c>
+      <c r="R3">
+        <v>6</v>
+      </c>
+      <c r="S3">
+        <v>7</v>
+      </c>
+      <c r="T3">
+        <v>8</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>10</v>
+      </c>
+      <c r="W3">
+        <v>2.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1151FF97-D0E1-0C4A-B3E8-5F557C369670}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1366,7 +1724,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1375,7 +1733,7 @@
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
         <v>39</v>
@@ -1384,7 +1742,7 @@
         <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1412,7 +1770,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1421,7 +1779,7 @@
         <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
         <v>39</v>
@@ -1430,7 +1788,7 @@
         <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1458,7 +1816,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1467,7 +1825,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
         <v>39</v>
@@ -1476,7 +1834,7 @@
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1484,12 +1842,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B613047-F522-7940-BBE5-BABC26E5D272}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:G18"/>
+      <selection activeCell="A14" activeCellId="1" sqref="A4:H4 A14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1504,7 +1862,7 @@
     <col min="8" max="8" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -1527,7 +1885,7 @@
         <v>45</v>
       </c>
       <c r="H1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1584,7 +1942,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1593,16 +1951,16 @@
         <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
+        <v>39</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -1610,7 +1968,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1631,21 +1989,21 @@
         <v>41</v>
       </c>
       <c r="H5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>39</v>
@@ -1657,38 +2015,38 @@
         <v>41</v>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
+        <v>39</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="H7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1697,7 +2055,7 @@
         <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>39</v>
@@ -1714,7 +2072,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1723,7 +2081,7 @@
         <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>39</v>
@@ -1740,25 +2098,25 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
+        <v>39</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -1766,16 +2124,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
         <v>39</v>
@@ -1787,18 +2145,18 @@
         <v>41</v>
       </c>
       <c r="H11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1813,52 +2171,52 @@
         <v>41</v>
       </c>
       <c r="H12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
+        <v>39</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="H13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" t="s">
         <v>41</v>
       </c>
       <c r="G14" t="s">
@@ -1870,21 +2228,21 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" t="s">
         <v>41</v>
       </c>
       <c r="G15" t="s">
@@ -1896,25 +2254,25 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16">
-        <v>3</v>
+        <v>39</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -1922,16 +2280,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
         <v>39</v>
@@ -1943,12 +2301,12 @@
         <v>41</v>
       </c>
       <c r="H17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1957,7 +2315,7 @@
         <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
         <v>39</v>
@@ -1969,12 +2327,12 @@
         <v>41</v>
       </c>
       <c r="H18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1983,22 +2341,1121 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19">
-        <v>2</v>
+        <v>39</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G19" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="H19" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDB9334-8F56-FD47-AA9B-D960EB678BC9}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>50</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>60</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>60</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>60</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>50</v>
+      </c>
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>60</v>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>60</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37" t="s">
+        <v>60</v>
+      </c>
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding rec pulse runs
</commit_message>
<xml_diff>
--- a/input/OM_EM_Scenarios.xlsx
+++ b/input/OM_EM_Scenarios.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5B6888-F668-5B48-B811-EA362C0CB8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED6EB2E-C3F2-0D40-A5D2-331EB6F4E21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
+    <workbookView xWindow="3980" yWindow="2240" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{7DE04263-F460-4046-B781-542FFAD9869D}"/>
   </bookViews>
   <sheets>
     <sheet name="OM" sheetId="1" r:id="rId1"/>
     <sheet name="OM_TestCases" sheetId="6" r:id="rId2"/>
-    <sheet name="EM_Self_Tests" sheetId="2" r:id="rId3"/>
-    <sheet name="EM_Runs" sheetId="3" r:id="rId4"/>
-    <sheet name="EM_Runs_TVCont" sheetId="4" r:id="rId5"/>
+    <sheet name="OM_RecPulse" sheetId="7" r:id="rId3"/>
+    <sheet name="EM_Self_Tests" sheetId="2" r:id="rId4"/>
+    <sheet name="EM_Runs" sheetId="3" r:id="rId5"/>
+    <sheet name="EM_Runs_TVCont" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="125">
   <si>
     <t>Fast_LL_DatLow</t>
   </si>
@@ -174,9 +175,6 @@
     <t>OM_Application</t>
   </si>
   <si>
-    <t>Fast_LL_DatLow,Fast_LL_DatHigh,Slow_LL_DatLow,Slow_LL_DatHigh</t>
-  </si>
-  <si>
     <t>Random_Effects</t>
   </si>
   <si>
@@ -252,9 +250,6 @@
     <t>5_2Fl_GL</t>
   </si>
   <si>
-    <t>Fast_GL_DatLow,Fast_GL_DatHigh,Slow_GL_DatLow,Slow_GL_DatHigh</t>
-  </si>
-  <si>
     <t>Term_1Fl_ExpL_TVCont_0.5</t>
   </si>
   <si>
@@ -388,6 +383,39 @@
   </si>
   <si>
     <t>ShortFast_GL_DatHigh</t>
+  </si>
+  <si>
+    <t>RecPulse_Fast_LL_DatLow</t>
+  </si>
+  <si>
+    <t>RecPulse_Fast_LL_DatHigh</t>
+  </si>
+  <si>
+    <t>RecPulse_Fast_GL_DatLow</t>
+  </si>
+  <si>
+    <t>RecPulse_Fast_GL_DatHigh</t>
+  </si>
+  <si>
+    <t>RecPulse_Slow_LL_DatLow</t>
+  </si>
+  <si>
+    <t>RecPulse_Slow_LL_DatHigh</t>
+  </si>
+  <si>
+    <t>RecPulse_Slow_GL_DatLow</t>
+  </si>
+  <si>
+    <t>RecPulse_Slow_GL_DatHigh</t>
+  </si>
+  <si>
+    <t>Fl_Chg_Rec_Pulse</t>
+  </si>
+  <si>
+    <t>Fast_LL_DatLow,Fast_LL_DatHigh,Slow_LL_DatLow,Slow_LL_DatHigh,RecPulse_Fast_LL_DatLow,RecPulse_Fast_LL_DatHigh,RecPulse_Slow_LL_DatLow,RecPulse_Slow_LL_DatHigh</t>
+  </si>
+  <si>
+    <t>Fast_GL_DatLow,Fast_GL_DatHigh,Slow_GL_DatLow,Slow_GL_DatHigh,RecPulse_Fast_GL_DatLow,RecPulse_Fast_GL_DatHigh,RecPulse_Slow_GL_DatLow,RecPulse_Slow_GL_DatHigh</t>
   </si>
 </sst>
 </file>
@@ -436,9 +464,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,7 +787,7 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" activeCellId="1" sqref="A3:XFD3 A5:XFD5"/>
+      <selection sqref="A1:W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -996,7 +1027,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -1067,7 +1098,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -1280,7 +1311,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1351,7 +1382,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -1429,7 +1460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79EC034-2FE7-9043-9DC4-2D3AB80C9B4B}">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -1513,7 +1544,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -1584,7 +1615,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1659,11 +1690,692 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A375176-8ABA-8045-B4C7-335203C533A3}">
+  <dimension ref="A1:X9"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>0.108</v>
+      </c>
+      <c r="E2">
+        <v>1.08E-3</v>
+      </c>
+      <c r="F2">
+        <v>0.01</v>
+      </c>
+      <c r="G2">
+        <v>0.85</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2">
+        <v>30</v>
+      </c>
+      <c r="J2">
+        <v>30</v>
+      </c>
+      <c r="K2">
+        <v>0.6</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2">
+        <v>4</v>
+      </c>
+      <c r="Q2">
+        <v>0.85</v>
+      </c>
+      <c r="R2">
+        <v>6</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>8</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2">
+        <v>10</v>
+      </c>
+      <c r="W2">
+        <v>2.5</v>
+      </c>
+      <c r="X2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>0.108</v>
+      </c>
+      <c r="E3">
+        <v>1.08E-3</v>
+      </c>
+      <c r="F3">
+        <v>0.01</v>
+      </c>
+      <c r="G3">
+        <v>0.85</v>
+      </c>
+      <c r="H3">
+        <v>200</v>
+      </c>
+      <c r="I3">
+        <v>200</v>
+      </c>
+      <c r="J3">
+        <v>200</v>
+      </c>
+      <c r="K3">
+        <v>0.2</v>
+      </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="M3">
+        <v>50</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>0.85</v>
+      </c>
+      <c r="R3">
+        <v>6</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>8</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>10</v>
+      </c>
+      <c r="W3">
+        <v>2.5</v>
+      </c>
+      <c r="X3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>0.108</v>
+      </c>
+      <c r="E4">
+        <v>1.08E-3</v>
+      </c>
+      <c r="F4">
+        <v>0.01</v>
+      </c>
+      <c r="G4">
+        <v>0.85</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>30</v>
+      </c>
+      <c r="J4">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>0.6</v>
+      </c>
+      <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>20</v>
+      </c>
+      <c r="N4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4">
+        <v>4</v>
+      </c>
+      <c r="Q4">
+        <v>6</v>
+      </c>
+      <c r="R4">
+        <v>6</v>
+      </c>
+      <c r="S4">
+        <v>7</v>
+      </c>
+      <c r="T4">
+        <v>8</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="V4">
+        <v>10</v>
+      </c>
+      <c r="W4">
+        <v>2.5</v>
+      </c>
+      <c r="X4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>0.108</v>
+      </c>
+      <c r="E5">
+        <v>1.08E-3</v>
+      </c>
+      <c r="F5">
+        <v>0.01</v>
+      </c>
+      <c r="G5">
+        <v>0.85</v>
+      </c>
+      <c r="H5">
+        <v>200</v>
+      </c>
+      <c r="I5">
+        <v>200</v>
+      </c>
+      <c r="J5">
+        <v>200</v>
+      </c>
+      <c r="K5">
+        <v>0.2</v>
+      </c>
+      <c r="L5">
+        <v>50</v>
+      </c>
+      <c r="M5">
+        <v>50</v>
+      </c>
+      <c r="N5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>6</v>
+      </c>
+      <c r="R5">
+        <v>6</v>
+      </c>
+      <c r="S5">
+        <v>7</v>
+      </c>
+      <c r="T5">
+        <v>8</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+      <c r="V5">
+        <v>10</v>
+      </c>
+      <c r="W5">
+        <v>2.5</v>
+      </c>
+      <c r="X5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>0.108</v>
+      </c>
+      <c r="E6">
+        <v>1.08E-3</v>
+      </c>
+      <c r="F6">
+        <v>0.01</v>
+      </c>
+      <c r="G6">
+        <v>0.85</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+      <c r="I6">
+        <v>30</v>
+      </c>
+      <c r="J6">
+        <v>30</v>
+      </c>
+      <c r="K6">
+        <v>0.6</v>
+      </c>
+      <c r="L6">
+        <v>20</v>
+      </c>
+      <c r="M6">
+        <v>20</v>
+      </c>
+      <c r="N6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="Q6">
+        <v>0.85</v>
+      </c>
+      <c r="R6">
+        <v>6</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>8</v>
+      </c>
+      <c r="U6">
+        <v>2</v>
+      </c>
+      <c r="V6">
+        <v>10</v>
+      </c>
+      <c r="W6">
+        <v>2.5</v>
+      </c>
+      <c r="X6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>0.108</v>
+      </c>
+      <c r="E7">
+        <v>1.08E-3</v>
+      </c>
+      <c r="F7">
+        <v>0.01</v>
+      </c>
+      <c r="G7">
+        <v>0.85</v>
+      </c>
+      <c r="H7">
+        <v>200</v>
+      </c>
+      <c r="I7">
+        <v>200</v>
+      </c>
+      <c r="J7">
+        <v>200</v>
+      </c>
+      <c r="K7">
+        <v>0.2</v>
+      </c>
+      <c r="L7">
+        <v>50</v>
+      </c>
+      <c r="M7">
+        <v>50</v>
+      </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7">
+        <v>4</v>
+      </c>
+      <c r="Q7">
+        <v>0.85</v>
+      </c>
+      <c r="R7">
+        <v>6</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>8</v>
+      </c>
+      <c r="U7">
+        <v>2</v>
+      </c>
+      <c r="V7">
+        <v>10</v>
+      </c>
+      <c r="W7">
+        <v>2.5</v>
+      </c>
+      <c r="X7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>0.108</v>
+      </c>
+      <c r="E8">
+        <v>1.08E-3</v>
+      </c>
+      <c r="F8">
+        <v>0.01</v>
+      </c>
+      <c r="G8">
+        <v>0.85</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <v>0.6</v>
+      </c>
+      <c r="L8">
+        <v>20</v>
+      </c>
+      <c r="M8">
+        <v>20</v>
+      </c>
+      <c r="N8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P8">
+        <v>4</v>
+      </c>
+      <c r="Q8">
+        <v>6</v>
+      </c>
+      <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
+      <c r="T8">
+        <v>8</v>
+      </c>
+      <c r="U8">
+        <v>2</v>
+      </c>
+      <c r="V8">
+        <v>10</v>
+      </c>
+      <c r="W8">
+        <v>2.5</v>
+      </c>
+      <c r="X8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>0.108</v>
+      </c>
+      <c r="E9">
+        <v>1.08E-3</v>
+      </c>
+      <c r="F9">
+        <v>0.01</v>
+      </c>
+      <c r="G9">
+        <v>0.85</v>
+      </c>
+      <c r="H9">
+        <v>200</v>
+      </c>
+      <c r="I9">
+        <v>200</v>
+      </c>
+      <c r="J9">
+        <v>200</v>
+      </c>
+      <c r="K9">
+        <v>0.2</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
+      </c>
+      <c r="M9">
+        <v>50</v>
+      </c>
+      <c r="N9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9">
+        <v>4</v>
+      </c>
+      <c r="Q9">
+        <v>6</v>
+      </c>
+      <c r="R9">
+        <v>6</v>
+      </c>
+      <c r="S9">
+        <v>7</v>
+      </c>
+      <c r="T9">
+        <v>8</v>
+      </c>
+      <c r="U9">
+        <v>2</v>
+      </c>
+      <c r="V9">
+        <v>10</v>
+      </c>
+      <c r="W9">
+        <v>2.5</v>
+      </c>
+      <c r="X9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1151FF97-D0E1-0C4A-B3E8-5F557C369670}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1699,7 +2411,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1718,13 +2430,13 @@
       <c r="F2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1733,7 +2445,7 @@
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
         <v>39</v>
@@ -1741,11 +2453,11 @@
       <c r="F3" t="s">
         <v>41</v>
       </c>
-      <c r="G3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1764,13 +2476,13 @@
       <c r="F4" t="s">
         <v>41</v>
       </c>
-      <c r="G4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1779,7 +2491,7 @@
         <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
         <v>39</v>
@@ -1787,11 +2499,11 @@
       <c r="F5" t="s">
         <v>41</v>
       </c>
-      <c r="G5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1810,13 +2522,13 @@
       <c r="F6" t="s">
         <v>41</v>
       </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1825,7 +2537,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
         <v>39</v>
@@ -1833,8 +2545,8 @@
       <c r="F7" t="s">
         <v>41</v>
       </c>
-      <c r="G7" t="s">
-        <v>70</v>
+      <c r="G7" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1842,12 +2554,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B613047-F522-7940-BBE5-BABC26E5D272}">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" activeCellId="1" sqref="A4:H4 A14:H14"/>
+      <selection activeCell="H19" sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1882,15 +2594,15 @@
         <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1899,7 +2611,7 @@
         <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
@@ -1916,7 +2628,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1925,7 +2637,7 @@
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>39</v>
@@ -1942,7 +2654,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1968,7 +2680,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1994,7 +2706,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2003,7 +2715,7 @@
         <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
         <v>39</v>
@@ -2020,7 +2732,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2029,7 +2741,7 @@
         <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
         <v>39</v>
@@ -2046,7 +2758,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2072,7 +2784,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2098,7 +2810,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2107,7 +2819,7 @@
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>39</v>
@@ -2124,7 +2836,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2133,7 +2845,7 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
         <v>39</v>
@@ -2150,7 +2862,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2176,7 +2888,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2202,7 +2914,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2228,7 +2940,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2254,7 +2966,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2280,7 +2992,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2306,7 +3018,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2332,7 +3044,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2364,12 +3076,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDB9334-8F56-FD47-AA9B-D960EB678BC9}">
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2401,18 +3113,18 @@
         <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2421,16 +3133,16 @@
         <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -2441,7 +3153,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2453,13 +3165,13 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -2470,7 +3182,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2479,16 +3191,16 @@
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -2499,7 +3211,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2511,13 +3223,13 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -2528,7 +3240,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2537,16 +3249,16 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -2557,7 +3269,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2569,13 +3281,13 @@
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -2586,7 +3298,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2595,16 +3307,16 @@
         <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8">
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -2615,7 +3327,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2627,13 +3339,13 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -2644,7 +3356,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2653,16 +3365,16 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10">
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -2673,7 +3385,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2685,13 +3397,13 @@
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -2702,7 +3414,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2711,16 +3423,16 @@
         <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F12">
         <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -2731,7 +3443,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2743,13 +3455,13 @@
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -2760,7 +3472,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2769,16 +3481,16 @@
         <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14">
         <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -2789,7 +3501,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2801,13 +3513,13 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -2818,7 +3530,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2827,16 +3539,16 @@
         <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F16">
         <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -2847,7 +3559,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2859,13 +3571,13 @@
         <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
@@ -2876,7 +3588,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2885,16 +3597,16 @@
         <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18">
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -2905,7 +3617,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2917,13 +3629,13 @@
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19">
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -2934,7 +3646,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2943,16 +3655,16 @@
         <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20">
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -2963,7 +3675,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2975,13 +3687,13 @@
         <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -2992,7 +3704,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3001,16 +3713,16 @@
         <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F22">
         <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
@@ -3021,7 +3733,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3033,13 +3745,13 @@
         <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23">
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
@@ -3050,7 +3762,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3059,16 +3771,16 @@
         <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F24">
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H24" t="b">
         <v>0</v>
@@ -3079,7 +3791,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3091,13 +3803,13 @@
         <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25">
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -3108,7 +3820,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3120,13 +3832,13 @@
         <v>15</v>
       </c>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26">
         <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H26" t="b">
         <v>0</v>
@@ -3137,7 +3849,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3149,13 +3861,13 @@
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F27">
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
@@ -3166,7 +3878,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3178,13 +3890,13 @@
         <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F28">
         <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H28" t="b">
         <v>0</v>
@@ -3195,7 +3907,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3207,13 +3919,13 @@
         <v>15</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29">
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
@@ -3224,7 +3936,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3236,13 +3948,13 @@
         <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30">
         <v>2</v>
       </c>
       <c r="G30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H30" t="b">
         <v>0</v>
@@ -3253,7 +3965,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3265,13 +3977,13 @@
         <v>15</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F31">
         <v>2</v>
       </c>
       <c r="G31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H31" t="b">
         <v>0</v>
@@ -3282,7 +3994,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3294,13 +4006,13 @@
         <v>15</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32">
         <v>2</v>
       </c>
       <c r="G32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H32" t="b">
         <v>0</v>
@@ -3311,7 +4023,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -3323,13 +4035,13 @@
         <v>15</v>
       </c>
       <c r="E33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33">
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
@@ -3340,7 +4052,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -3352,13 +4064,13 @@
         <v>15</v>
       </c>
       <c r="E34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F34">
         <v>2</v>
       </c>
       <c r="G34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
@@ -3369,7 +4081,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -3381,13 +4093,13 @@
         <v>15</v>
       </c>
       <c r="E35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F35">
         <v>2</v>
       </c>
       <c r="G35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
@@ -3398,7 +4110,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -3410,13 +4122,13 @@
         <v>15</v>
       </c>
       <c r="E36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F36">
         <v>2</v>
       </c>
       <c r="G36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H36" t="b">
         <v>0</v>
@@ -3427,7 +4139,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -3439,13 +4151,13 @@
         <v>15</v>
       </c>
       <c r="E37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F37">
         <v>2</v>
       </c>
       <c r="G37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H37" t="b">
         <v>0</v>

</xml_diff>